<commit_message>
Clase 9 de programación
</commit_message>
<xml_diff>
--- a/Apuntes/Clase8_ActividadProcesos2.xlsx
+++ b/Apuntes/Clase8_ActividadProcesos2.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexa\Documents\DH\1°Bimestre\II\Apuntes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6D016B-08FE-4CD9-B876-82B8EE676D58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="FIFO" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="SJF" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="SRTF" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Round Robin (Q=1)" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Round Robin (Q=2)" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Round Robin (Q=4)" sheetId="6" r:id="rId9"/>
+    <sheet name="FIFO" sheetId="1" r:id="rId1"/>
+    <sheet name="SJF" sheetId="2" r:id="rId2"/>
+    <sheet name="SRTF" sheetId="3" r:id="rId3"/>
+    <sheet name="Round Robin (Q=1)" sheetId="4" r:id="rId4"/>
+    <sheet name="Round Robin (Q=2)" sheetId="5" r:id="rId5"/>
+    <sheet name="Round Robin (Q=4)" sheetId="6" r:id="rId6"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -51,43 +60,55 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FFFF00FF"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFFF00FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <strike/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <i/>
       <strike/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -137,127 +158,146 @@
         <bgColor theme="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
-    <border/>
+  <borders count="7">
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="31">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -447,27 +487,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.0"/>
-    <col customWidth="1" min="2" max="2" width="7.57"/>
-    <col customWidth="1" min="3" max="3" width="15.14"/>
-    <col customWidth="1" min="4" max="23" width="4.57"/>
-    <col customWidth="1" min="24" max="24" width="5.0"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="7.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.08984375" customWidth="1"/>
+    <col min="4" max="23" width="4.54296875" customWidth="1"/>
+    <col min="24" max="24" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,62 +521,62 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
@@ -541,7 +584,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
@@ -552,7 +595,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
@@ -561,7 +604,7 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
@@ -571,14 +614,14 @@
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -601,80 +644,82 @@
       <c r="W14" s="13"/>
       <c r="X14" s="13"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="15">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E15" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="16">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="16">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H15" s="16">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I15" s="16">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J15" s="16">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="K15" s="16">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="L15" s="16">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="M15" s="16">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="N15" s="16">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="O15" s="16">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="P15" s="16">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="Q15" s="16">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="R15" s="16">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="S15" s="16">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="T15" s="16">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="U15" s="16">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="V15" s="16">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="W15" s="16">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="X15" s="16">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+    </row>
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -698,10 +743,10 @@
       <c r="W19" s="17"/>
       <c r="X19" s="17"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="17"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
         <v>3</v>
       </c>
@@ -709,7 +754,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
         <v>4</v>
       </c>
@@ -720,7 +765,7 @@
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
         <v>5</v>
       </c>
@@ -731,7 +776,7 @@
       <c r="V23" s="18"/>
       <c r="W23" s="18"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
@@ -741,7 +786,7 @@
       <c r="T24" s="11"/>
       <c r="U24" s="11"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>7</v>
       </c>
@@ -767,7 +812,7 @@
       <c r="W25" s="19"/>
       <c r="X25" s="17"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
@@ -790,99 +835,100 @@
       <c r="W26" s="17"/>
       <c r="X26" s="17"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C27" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="20">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E27" s="21">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="21">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G27" s="21">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H27" s="21">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I27" s="21">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J27" s="21">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="K27" s="21">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="L27" s="21">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="M27" s="21">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="N27" s="21">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="O27" s="21">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="P27" s="21">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="Q27" s="21">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="R27" s="21">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="S27" s="21">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="T27" s="21">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="U27" s="21">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="V27" s="21">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="W27" s="21">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="X27" s="21">
-        <v>20.0</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A18:C18"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.0"/>
-    <col customWidth="1" min="2" max="2" width="7.57"/>
-    <col customWidth="1" min="3" max="3" width="15.14"/>
-    <col customWidth="1" min="4" max="24" width="4.71"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="7.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.08984375" customWidth="1"/>
+    <col min="4" max="24" width="4.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -893,62 +939,62 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
@@ -956,7 +1002,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
@@ -967,7 +1013,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
@@ -976,7 +1022,7 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
@@ -986,14 +1032,14 @@
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -1016,87 +1062,89 @@
       <c r="W14" s="13"/>
       <c r="X14" s="13"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="15">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E15" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="16">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="16">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H15" s="16">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I15" s="16">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J15" s="16">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="K15" s="16">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="L15" s="16">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="M15" s="16">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="N15" s="16">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="O15" s="16">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="P15" s="16">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="Q15" s="16">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="R15" s="16">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="S15" s="16">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="T15" s="16">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="U15" s="16">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="V15" s="16">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="W15" s="16">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="X15" s="16">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+    </row>
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="17"/>
       <c r="X19" s="17"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="17"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
         <v>3</v>
       </c>
@@ -1104,7 +1152,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
         <v>4</v>
       </c>
@@ -1115,7 +1163,7 @@
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
         <v>5</v>
       </c>
@@ -1126,7 +1174,7 @@
       <c r="V23" s="22"/>
       <c r="W23" s="22"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
@@ -1136,7 +1184,7 @@
       <c r="V24" s="11"/>
       <c r="W24" s="11"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1144,7 +1192,7 @@
       <c r="N25" s="12"/>
       <c r="X25" s="17"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
@@ -1167,99 +1215,102 @@
       <c r="W26" s="17"/>
       <c r="X26" s="17"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C27" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="20">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E27" s="21">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="21">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G27" s="21">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H27" s="21">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I27" s="21">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J27" s="21">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="K27" s="21">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="L27" s="21">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="M27" s="21">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="N27" s="21">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="O27" s="21">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="P27" s="21">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="Q27" s="21">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="R27" s="21">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="S27" s="21">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="T27" s="21">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="U27" s="21">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="V27" s="21">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="W27" s="21">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="X27" s="21">
-        <v>20.0</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A18:C18"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Y23" sqref="Y23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.0"/>
-    <col customWidth="1" min="2" max="2" width="7.57"/>
-    <col customWidth="1" min="3" max="3" width="15.14"/>
-    <col customWidth="1" min="4" max="24" width="4.57"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="7.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.08984375" customWidth="1"/>
+    <col min="4" max="24" width="4.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1270,62 +1321,62 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1333,7 +1384,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
@@ -1344,7 +1395,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
@@ -1353,7 +1404,7 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1363,14 +1414,14 @@
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -1393,80 +1444,82 @@
       <c r="W14" s="13"/>
       <c r="X14" s="13"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="15">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E15" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="16">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="16">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H15" s="16">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I15" s="16">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J15" s="16">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="K15" s="16">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="L15" s="16">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="M15" s="16">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="N15" s="16">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="O15" s="16">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="P15" s="16">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="Q15" s="16">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="R15" s="16">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="S15" s="16">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="T15" s="16">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="U15" s="16">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="V15" s="16">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="W15" s="16">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="X15" s="16">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+    </row>
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -1490,10 +1543,10 @@
       <c r="W19" s="17"/>
       <c r="X19" s="17"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="17"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
         <v>3</v>
       </c>
@@ -1501,7 +1554,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
         <v>4</v>
       </c>
@@ -1512,7 +1565,7 @@
       <c r="Q22" s="9"/>
       <c r="R22" s="9"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
         <v>5</v>
       </c>
@@ -1523,7 +1576,7 @@
       <c r="V23" s="22"/>
       <c r="W23" s="22"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
@@ -1533,14 +1586,14 @@
       <c r="V24" s="11"/>
       <c r="W24" s="11"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>7</v>
       </c>
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
@@ -1563,99 +1616,102 @@
       <c r="W26" s="17"/>
       <c r="X26" s="17"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C27" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="E27" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="F27" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="G27" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="H27" s="16">
-        <v>4.0</v>
-      </c>
-      <c r="I27" s="16">
-        <v>5.0</v>
-      </c>
-      <c r="J27" s="16">
-        <v>6.0</v>
-      </c>
-      <c r="K27" s="16">
-        <v>7.0</v>
-      </c>
-      <c r="L27" s="16">
-        <v>8.0</v>
-      </c>
-      <c r="M27" s="16">
-        <v>9.0</v>
-      </c>
-      <c r="N27" s="16">
-        <v>10.0</v>
-      </c>
-      <c r="O27" s="16">
-        <v>11.0</v>
-      </c>
-      <c r="P27" s="16">
-        <v>12.0</v>
-      </c>
-      <c r="Q27" s="16">
-        <v>13.0</v>
-      </c>
-      <c r="R27" s="16">
-        <v>14.0</v>
-      </c>
-      <c r="S27" s="16">
-        <v>15.0</v>
-      </c>
-      <c r="T27" s="16">
-        <v>16.0</v>
-      </c>
-      <c r="U27" s="16">
-        <v>17.0</v>
-      </c>
-      <c r="V27" s="16">
-        <v>18.0</v>
-      </c>
-      <c r="W27" s="16">
-        <v>19.0</v>
-      </c>
-      <c r="X27" s="16">
-        <v>20.0</v>
+      <c r="D27" s="29">
+        <v>0</v>
+      </c>
+      <c r="E27" s="30">
+        <v>1</v>
+      </c>
+      <c r="F27" s="30">
+        <v>2</v>
+      </c>
+      <c r="G27" s="30">
+        <v>3</v>
+      </c>
+      <c r="H27" s="30">
+        <v>4</v>
+      </c>
+      <c r="I27" s="30">
+        <v>5</v>
+      </c>
+      <c r="J27" s="30">
+        <v>6</v>
+      </c>
+      <c r="K27" s="30">
+        <v>7</v>
+      </c>
+      <c r="L27" s="30">
+        <v>8</v>
+      </c>
+      <c r="M27" s="30">
+        <v>9</v>
+      </c>
+      <c r="N27" s="30">
+        <v>10</v>
+      </c>
+      <c r="O27" s="30">
+        <v>11</v>
+      </c>
+      <c r="P27" s="30">
+        <v>12</v>
+      </c>
+      <c r="Q27" s="30">
+        <v>13</v>
+      </c>
+      <c r="R27" s="30">
+        <v>14</v>
+      </c>
+      <c r="S27" s="30">
+        <v>15</v>
+      </c>
+      <c r="T27" s="30">
+        <v>16</v>
+      </c>
+      <c r="U27" s="30">
+        <v>17</v>
+      </c>
+      <c r="V27" s="30">
+        <v>18</v>
+      </c>
+      <c r="W27" s="30">
+        <v>19</v>
+      </c>
+      <c r="X27" s="30">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A18:C18"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:X32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.0"/>
-    <col customWidth="1" min="2" max="2" width="7.57"/>
-    <col customWidth="1" min="3" max="3" width="10.71"/>
-    <col customWidth="1" min="4" max="24" width="5.71"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="7.54296875" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" customWidth="1"/>
+    <col min="4" max="24" width="5.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1666,62 +1722,62 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
@@ -1729,7 +1785,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
@@ -1740,7 +1796,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
@@ -1749,7 +1805,7 @@
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
@@ -1759,14 +1815,14 @@
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -1789,80 +1845,553 @@
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="15">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E16" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="16">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G16" s="16">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H16" s="16">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I16" s="16">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J16" s="16">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="K16" s="16">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="L16" s="16">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="M16" s="16">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="N16" s="16">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="O16" s="16">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="P16" s="16">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="Q16" s="16">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="R16" s="16">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="S16" s="16">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="T16" s="16">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="U16" s="16">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="V16" s="16">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="W16" s="16">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="X16" s="16">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20">
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+    </row>
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="17"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="17"/>
+    </row>
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="17"/>
+    </row>
+    <row r="22" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="U23" s="9"/>
+    </row>
+    <row r="24" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="V24" s="18"/>
+      <c r="W24" s="18"/>
+    </row>
+    <row r="25" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+    </row>
+    <row r="26" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="23"/>
+      <c r="U26" s="23"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="17"/>
+    </row>
+    <row r="27" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="23"/>
+      <c r="U27" s="17"/>
+      <c r="V27" s="17"/>
+      <c r="W27" s="17"/>
+      <c r="X27" s="17"/>
+    </row>
+    <row r="28" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C28" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="20">
+        <v>0</v>
+      </c>
+      <c r="E28" s="21">
+        <v>1</v>
+      </c>
+      <c r="F28" s="21">
+        <v>2</v>
+      </c>
+      <c r="G28" s="21">
+        <v>3</v>
+      </c>
+      <c r="H28" s="21">
+        <v>4</v>
+      </c>
+      <c r="I28" s="21">
+        <v>5</v>
+      </c>
+      <c r="J28" s="21">
+        <v>6</v>
+      </c>
+      <c r="K28" s="21">
+        <v>7</v>
+      </c>
+      <c r="L28" s="21">
+        <v>8</v>
+      </c>
+      <c r="M28" s="21">
+        <v>9</v>
+      </c>
+      <c r="N28" s="21">
+        <v>10</v>
+      </c>
+      <c r="O28" s="21">
+        <v>11</v>
+      </c>
+      <c r="P28" s="21">
+        <v>12</v>
+      </c>
+      <c r="Q28" s="21">
+        <v>13</v>
+      </c>
+      <c r="R28" s="21">
+        <v>14</v>
+      </c>
+      <c r="S28" s="21">
+        <v>15</v>
+      </c>
+      <c r="T28" s="21">
+        <v>16</v>
+      </c>
+      <c r="U28" s="21">
+        <v>17</v>
+      </c>
+      <c r="V28" s="21">
+        <v>18</v>
+      </c>
+      <c r="W28" s="21">
+        <v>19</v>
+      </c>
+      <c r="X28" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="13" x14ac:dyDescent="0.3">
+      <c r="F29" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="J29" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="F30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="F31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="J32" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A19:C19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:X28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="7.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.08984375" customWidth="1"/>
+    <col min="4" max="24" width="4.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+    </row>
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+    </row>
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+    </row>
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="15">
+        <v>0</v>
+      </c>
+      <c r="E16" s="16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="16">
+        <v>2</v>
+      </c>
+      <c r="G16" s="16">
+        <v>3</v>
+      </c>
+      <c r="H16" s="16">
+        <v>4</v>
+      </c>
+      <c r="I16" s="16">
+        <v>5</v>
+      </c>
+      <c r="J16" s="16">
+        <v>6</v>
+      </c>
+      <c r="K16" s="16">
+        <v>7</v>
+      </c>
+      <c r="L16" s="16">
+        <v>8</v>
+      </c>
+      <c r="M16" s="16">
+        <v>9</v>
+      </c>
+      <c r="N16" s="16">
+        <v>10</v>
+      </c>
+      <c r="O16" s="16">
+        <v>11</v>
+      </c>
+      <c r="P16" s="16">
+        <v>12</v>
+      </c>
+      <c r="Q16" s="16">
+        <v>13</v>
+      </c>
+      <c r="R16" s="16">
+        <v>14</v>
+      </c>
+      <c r="S16" s="16">
+        <v>15</v>
+      </c>
+      <c r="T16" s="16">
+        <v>16</v>
+      </c>
+      <c r="U16" s="16">
+        <v>17</v>
+      </c>
+      <c r="V16" s="16">
+        <v>18</v>
+      </c>
+      <c r="W16" s="16">
+        <v>19</v>
+      </c>
+      <c r="X16" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+    </row>
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
@@ -1886,76 +2415,67 @@
       <c r="W20" s="17"/>
       <c r="X20" s="17"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="17"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23">
+      <c r="H22" s="8"/>
+    </row>
+    <row r="23" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="U23" s="9"/>
-    </row>
-    <row r="24">
+      <c r="G23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+    </row>
+    <row r="24" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I24" s="10"/>
-      <c r="L24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="O24" s="10"/>
       <c r="P24" s="10"/>
-      <c r="T24" s="10"/>
       <c r="V24" s="18"/>
       <c r="W24" s="18"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="S25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="U25" s="11"/>
       <c r="V25" s="11"/>
       <c r="W25" s="11"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
       <c r="M26" s="17"/>
-      <c r="N26" s="19"/>
+      <c r="N26" s="17"/>
       <c r="O26" s="17"/>
       <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
+      <c r="Q26" s="19"/>
       <c r="R26" s="19"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="17"/>
+      <c r="U26" s="17"/>
       <c r="V26" s="17"/>
       <c r="W26" s="17"/>
       <c r="X26" s="17"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
@@ -1972,158 +2492,106 @@
       <c r="Q27" s="17"/>
       <c r="R27" s="17"/>
       <c r="S27" s="17"/>
-      <c r="T27" s="23"/>
+      <c r="T27" s="17"/>
       <c r="U27" s="17"/>
       <c r="V27" s="17"/>
       <c r="W27" s="17"/>
       <c r="X27" s="17"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C28" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="20">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E28" s="21">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="21">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G28" s="21">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H28" s="21">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I28" s="21">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J28" s="21">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="K28" s="21">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="L28" s="21">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="M28" s="21">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="N28" s="21">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="O28" s="21">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="P28" s="21">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="Q28" s="21">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="R28" s="21">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="S28" s="21">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="T28" s="21">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="U28" s="21">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="V28" s="21">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="W28" s="21">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="X28" s="21">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="F29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="G29" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="H29" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="I29" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="J29" s="24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="F30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="F31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="J32" s="3" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A19:C19"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:X28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.0"/>
-    <col customWidth="1" min="2" max="2" width="7.57"/>
-    <col customWidth="1" min="3" max="3" width="15.14"/>
-    <col customWidth="1" min="4" max="24" width="4.86"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="7.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.08984375" customWidth="1"/>
+    <col min="4" max="24" width="5.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2134,62 +2602,62 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
@@ -2197,7 +2665,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
@@ -2208,7 +2676,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
@@ -2217,7 +2685,7 @@
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
@@ -2227,14 +2695,14 @@
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -2257,90 +2725,83 @@
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="15">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E16" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="16">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G16" s="16">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H16" s="16">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I16" s="16">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J16" s="16">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="K16" s="16">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="L16" s="16">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="M16" s="16">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="N16" s="16">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="O16" s="16">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="P16" s="16">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="Q16" s="16">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="R16" s="16">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="S16" s="16">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="T16" s="16">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="U16" s="16">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="V16" s="16">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="W16" s="16">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="X16" s="16">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20">
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+    </row>
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
       <c r="O20" s="17"/>
@@ -2354,67 +2815,76 @@
       <c r="W20" s="17"/>
       <c r="X20" s="17"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="17"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
-      <c r="H22" s="8"/>
-    </row>
-    <row r="23">
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-    </row>
-    <row r="24">
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+    </row>
+    <row r="24" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
       <c r="V24" s="18"/>
       <c r="W24" s="18"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
       <c r="W25" s="11"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
       <c r="O26" s="17"/>
       <c r="P26" s="17"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="19"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
       <c r="S26" s="17"/>
       <c r="T26" s="17"/>
-      <c r="U26" s="17"/>
-      <c r="V26" s="17"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="19"/>
       <c r="W26" s="17"/>
       <c r="X26" s="17"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
@@ -2437,484 +2907,78 @@
       <c r="W27" s="17"/>
       <c r="X27" s="17"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:24" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C28" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="20">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E28" s="21">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="21">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G28" s="21">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H28" s="21">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I28" s="21">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J28" s="21">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="K28" s="21">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="L28" s="21">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="M28" s="21">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="N28" s="21">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="O28" s="21">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="P28" s="21">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="Q28" s="21">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="R28" s="21">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="S28" s="21">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="T28" s="21">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="U28" s="21">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="V28" s="21">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="W28" s="21">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="X28" s="21">
-        <v>20.0</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A19:C19"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="9.0"/>
-    <col customWidth="1" min="2" max="2" width="7.57"/>
-    <col customWidth="1" min="3" max="3" width="15.14"/>
-    <col customWidth="1" min="4" max="24" width="5.71"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3">
-        <v>6.0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3">
-        <v>8.0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="C10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11">
-      <c r="C11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-    </row>
-    <row r="12">
-      <c r="C12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-    </row>
-    <row r="13">
-      <c r="C13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-    </row>
-    <row r="14">
-      <c r="C14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-    </row>
-    <row r="15">
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
-      <c r="V15" s="13"/>
-      <c r="W15" s="13"/>
-      <c r="X15" s="13"/>
-    </row>
-    <row r="16">
-      <c r="C16" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="E16" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="F16" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="G16" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="H16" s="16">
-        <v>4.0</v>
-      </c>
-      <c r="I16" s="16">
-        <v>5.0</v>
-      </c>
-      <c r="J16" s="16">
-        <v>6.0</v>
-      </c>
-      <c r="K16" s="16">
-        <v>7.0</v>
-      </c>
-      <c r="L16" s="16">
-        <v>8.0</v>
-      </c>
-      <c r="M16" s="16">
-        <v>9.0</v>
-      </c>
-      <c r="N16" s="16">
-        <v>10.0</v>
-      </c>
-      <c r="O16" s="16">
-        <v>11.0</v>
-      </c>
-      <c r="P16" s="16">
-        <v>12.0</v>
-      </c>
-      <c r="Q16" s="16">
-        <v>13.0</v>
-      </c>
-      <c r="R16" s="16">
-        <v>14.0</v>
-      </c>
-      <c r="S16" s="16">
-        <v>15.0</v>
-      </c>
-      <c r="T16" s="16">
-        <v>16.0</v>
-      </c>
-      <c r="U16" s="16">
-        <v>17.0</v>
-      </c>
-      <c r="V16" s="16">
-        <v>18.0</v>
-      </c>
-      <c r="W16" s="16">
-        <v>19.0</v>
-      </c>
-      <c r="X16" s="16">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="C20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
-      <c r="U20" s="17"/>
-      <c r="V20" s="17"/>
-      <c r="W20" s="17"/>
-      <c r="X20" s="17"/>
-    </row>
-    <row r="21">
-      <c r="C21" s="17"/>
-    </row>
-    <row r="22">
-      <c r="C22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23">
-      <c r="C23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-    </row>
-    <row r="24">
-      <c r="C24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="V24" s="18"/>
-      <c r="W24" s="18"/>
-    </row>
-    <row r="25">
-      <c r="C25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="W25" s="11"/>
-    </row>
-    <row r="26">
-      <c r="C26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="17"/>
-      <c r="S26" s="17"/>
-      <c r="T26" s="17"/>
-      <c r="U26" s="19"/>
-      <c r="V26" s="19"/>
-      <c r="W26" s="17"/>
-      <c r="X26" s="17"/>
-    </row>
-    <row r="27">
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="17"/>
-      <c r="S27" s="17"/>
-      <c r="T27" s="17"/>
-      <c r="U27" s="17"/>
-      <c r="V27" s="17"/>
-      <c r="W27" s="17"/>
-      <c r="X27" s="17"/>
-    </row>
-    <row r="28">
-      <c r="C28" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="E28" s="21">
-        <v>1.0</v>
-      </c>
-      <c r="F28" s="21">
-        <v>2.0</v>
-      </c>
-      <c r="G28" s="21">
-        <v>3.0</v>
-      </c>
-      <c r="H28" s="21">
-        <v>4.0</v>
-      </c>
-      <c r="I28" s="21">
-        <v>5.0</v>
-      </c>
-      <c r="J28" s="21">
-        <v>6.0</v>
-      </c>
-      <c r="K28" s="21">
-        <v>7.0</v>
-      </c>
-      <c r="L28" s="21">
-        <v>8.0</v>
-      </c>
-      <c r="M28" s="21">
-        <v>9.0</v>
-      </c>
-      <c r="N28" s="21">
-        <v>10.0</v>
-      </c>
-      <c r="O28" s="21">
-        <v>11.0</v>
-      </c>
-      <c r="P28" s="21">
-        <v>12.0</v>
-      </c>
-      <c r="Q28" s="21">
-        <v>13.0</v>
-      </c>
-      <c r="R28" s="21">
-        <v>14.0</v>
-      </c>
-      <c r="S28" s="21">
-        <v>15.0</v>
-      </c>
-      <c r="T28" s="21">
-        <v>16.0</v>
-      </c>
-      <c r="U28" s="21">
-        <v>17.0</v>
-      </c>
-      <c r="V28" s="21">
-        <v>18.0</v>
-      </c>
-      <c r="W28" s="21">
-        <v>19.0</v>
-      </c>
-      <c r="X28" s="21">
-        <v>20.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A19:C19"/>
-  </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>